<commit_message>
hay que continuar con la calculadora
</commit_message>
<xml_diff>
--- a/Servicios y procesos/Ejericico colas.xlsx
+++ b/Servicios y procesos/Ejericico colas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuh\Desktop\git\DAM2\Servicios y procesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0852C83F-5536-4B6D-B306-2331B2B34559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D592323-7E9A-4810-9EC3-E5AE826C1143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5A7FFB7-DF60-476E-B3B7-83AC55AC105A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="24">
   <si>
     <t>duracion</t>
   </si>
@@ -97,13 +98,25 @@
   </si>
   <si>
     <t>CC</t>
+  </si>
+  <si>
+    <t>Ejecucion</t>
+  </si>
+  <si>
+    <t>Bloqueado</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +132,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +159,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6969"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -168,16 +212,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6969"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -486,14 +539,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6AAE50-3C59-4E7A-90A0-335EE721DEB9}">
-  <dimension ref="A2:Q13"/>
+  <dimension ref="A2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
@@ -573,30 +627,30 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="I8" s="8"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="K9" s="7" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="K9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="O9" s="7" t="s">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="O9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -643,49 +697,49 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="L11">
         <v>3</v>
       </c>
       <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="P11">
         <v>4</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>100</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -693,32 +747,26 @@
       <c r="E12">
         <v>101</v>
       </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
+      <c r="G12" s="9"/>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K12" s="9"/>
       <c r="L12">
         <v>3</v>
       </c>
       <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O12" s="9"/>
       <c r="P12">
         <v>4</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -728,41 +776,1265 @@
       <c r="B13">
         <v>110</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
+      <c r="C13" s="9"/>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="E13">
         <v>101</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K13" s="9"/>
       <c r="L13">
         <v>2</v>
       </c>
       <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>18</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O13" s="9"/>
       <c r="P13">
         <v>3</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>210</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>101</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>101</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>220</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>101</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>101</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>320</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>101</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>101</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <v>101</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>330</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>101</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>101</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>101</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>430</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>101</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>101</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>101</v>
+      </c>
+      <c r="O18" s="9"/>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>440</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>101</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>101</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>101</v>
+      </c>
+      <c r="O19" s="9"/>
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>540</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>201</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>101</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>101</v>
+      </c>
+      <c r="O20" s="9"/>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>550</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>201</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>101</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>101</v>
+      </c>
+      <c r="O21" s="9"/>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>590</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>201</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I22">
+        <v>141</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>101</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>600</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>201</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I23">
+        <v>141</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>101</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>620</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>201</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I24">
+        <v>141</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24">
+        <v>-1120</v>
+      </c>
+      <c r="M24">
+        <v>121</v>
+      </c>
+      <c r="O24" s="9"/>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>630</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>201</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I25">
+        <v>141</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25">
+        <v>-1120</v>
+      </c>
+      <c r="M25">
+        <v>121</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>730</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>201</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I26">
+        <v>141</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26">
+        <v>-1120</v>
+      </c>
+      <c r="M26">
+        <v>121</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>740</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>201</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I27">
+        <v>141</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27">
+        <v>-1120</v>
+      </c>
+      <c r="M27">
+        <v>121</v>
+      </c>
+      <c r="O27" s="9"/>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>840</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>301</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I28">
+        <v>141</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28">
+        <v>-1120</v>
+      </c>
+      <c r="M28">
+        <v>121</v>
+      </c>
+      <c r="O28" s="9"/>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>850</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>301</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29">
+        <f>- (890)</f>
+        <v>-890</v>
+      </c>
+      <c r="I29">
+        <v>141</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29">
+        <v>-1120</v>
+      </c>
+      <c r="M29">
+        <v>121</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>890</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>301</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>141</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30">
+        <v>-1120</v>
+      </c>
+      <c r="M30">
+        <v>121</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <v>900</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>301</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>141</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31">
+        <v>-1120</v>
+      </c>
+      <c r="M31">
+        <v>121</v>
+      </c>
+      <c r="O31" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>1000</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>141</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32">
+        <v>-1120</v>
+      </c>
+      <c r="M32">
+        <v>121</v>
+      </c>
+      <c r="O32" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>1010</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>141</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33">
+        <v>-1120</v>
+      </c>
+      <c r="M33">
+        <v>121</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>1110</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>241</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34">
+        <v>-1120</v>
+      </c>
+      <c r="M34">
+        <v>121</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P34" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>1120</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>241</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>121</v>
+      </c>
+      <c r="O35" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P35" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>1220</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>341</v>
+      </c>
+      <c r="K36" s="9"/>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>121</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>1230</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>341</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>121</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>1330</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>341</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+      <c r="M38">
+        <v>221</v>
+      </c>
+      <c r="O38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>1340</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>341</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>221</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1440</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>441</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>221</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P40" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>1450</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>441</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>221</v>
+      </c>
+      <c r="O41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P41" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>1530</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>441</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L42" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P42" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>1540</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>441</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>1550</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L44" t="s">
+        <v>23</v>
+      </c>
+      <c r="M44" t="s">
+        <v>23</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P44" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>